<commit_message>
Added functionality to send Excel through email
</commit_message>
<xml_diff>
--- a/All Workshops Report.xlsx
+++ b/All Workshops Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ancoman/PycharmProjects/checkInvalidURLs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94E77145-D169-D14C-8F34-F227D1EBA20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D235D4C-C0BE-9440-B9FD-92D51CCA172A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="All Workshops Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -9336,7 +9337,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1270" sqref="D1270"/>
+      <selection pane="bottomLeft" activeCell="G1264" sqref="G1264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10537,10 +10538,10 @@
       <c r="F47" s="4">
         <v>44082</v>
       </c>
-      <c r="G47" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="H47" s="3"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="48" spans="1:8" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
@@ -40926,7 +40927,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G47" r:id="rId1" xr:uid="{70EA0306-4F8C-004B-A3F7-44A2227558AC}"/>
+    <hyperlink ref="H47" r:id="rId1" xr:uid="{905A067E-512C-C549-A00D-429C6CEDB295}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>